<commit_message>
Restful-booker: Major changes in Testcases
</commit_message>
<xml_diff>
--- a/target/test-classes/utilities/Activities_Data.xlsx
+++ b/target/test-classes/utilities/Activities_Data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Md Zinnun Uddin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Eclipse Projects\RestAssuredAPITesting\src\test\java\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="23040" windowHeight="9048"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="23040" windowHeight="9048"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>ID</t>
   </si>
@@ -48,12 +48,6 @@
   </si>
   <si>
     <t>baseball</t>
-  </si>
-  <si>
-    <t>hockey</t>
-  </si>
-  <si>
-    <t>2022-01-28T11:12:41.960Z</t>
   </si>
   <si>
     <t>2022-01-15T10:12:41.960Z</t>
@@ -443,11 +437,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -478,7 +470,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2" s="3" t="b">
         <v>1</v>
@@ -492,7 +484,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" s="3" t="b">
         <v>1</v>
@@ -506,7 +498,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" s="3" t="b">
         <v>1</v>
@@ -520,23 +512,9 @@
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D5" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="3" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>